<commit_message>
New script for quota status
</commit_message>
<xml_diff>
--- a/TestData/Custom_Quota_Status.xlsx
+++ b/TestData/Custom_Quota_Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neogis\D Drive\FREEDOM\Python\CloudAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D349DF-C220-4654-BD8C-4AF3418A8034}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B4D096-8944-4940-88D5-297120BA3286}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{458AF82A-ED03-4F93-994B-60962EF35F93}"/>
   </bookViews>
@@ -133,7 +133,7 @@
     <t>individualQuotaValuesId-row-3-colorQuota</t>
   </si>
   <si>
-    <t>Vary_Total5000_Color5000</t>
+    <t>Vary_Total6000_Color5000</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B209AA-B2EF-4EBA-BC33-9B6FB480ED25}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>